<commit_message>
refactor(all): add iesplan example
</commit_message>
<xml_diff>
--- a/mems/examples/iesplan/layout.xlsx
+++ b/mems/examples/iesplan/layout.xlsx
@@ -16,10 +16,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -38,6 +38,59 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -45,11 +98,49 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -60,9 +151,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -76,99 +166,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,13 +183,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -201,7 +279,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -213,157 +291,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -542,6 +542,15 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -562,39 +571,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -605,17 +581,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -638,8 +603,43 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -648,142 +648,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1167,30 +1167,30 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15" outlineLevelRow="5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="B1" s="2">
-        <v>2</v>
+        <v>600</v>
       </c>
       <c r="C1" s="2">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="D1" s="3">
-        <v>4</v>
+        <v>300</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="1">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="G1" s="3">
-        <v>6</v>
+        <v>300</v>
       </c>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
@@ -1200,14 +1200,14 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
       <c r="E2" s="10"/>
       <c r="F2" s="1">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="11"/>
@@ -1218,14 +1218,14 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="2">
-        <v>9</v>
+        <v>300</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="6"/>
       <c r="D3" s="7"/>
       <c r="E3" s="12"/>
       <c r="F3" s="1">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="13"/>
@@ -1238,16 +1238,16 @@
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="1">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="D4" s="1">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="E4" s="1">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="F4" s="14">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -1260,44 +1260,46 @@
       <c r="A5" s="6"/>
       <c r="B5" s="4"/>
       <c r="C5" s="1">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3"/>
+        <v>100</v>
+      </c>
+      <c r="D5" s="3">
+        <v>200</v>
+      </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="8"/>
       <c r="H5" s="1">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="I5" s="3">
-        <v>17</v>
+        <v>200</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="8"/>
       <c r="L5" s="1">
-        <v>18</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="1">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="12"/>
       <c r="H6" s="1">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="13"/>
       <c r="K6" s="12"/>
       <c r="L6" s="1">
-        <v>22</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>